<commit_message>
Sppring 2. Ver y eliminar tarjetas. Actualizacion docuemntacion pruebas
</commit_message>
<xml_diff>
--- a/documentacion/Test Manual/Testing Manual.xlsx
+++ b/documentacion/Test Manual/Testing Manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\OneDrive\Desktop\REPOSITORIO DIGITAL MONEY HOUSE\digital-money-house-backend\documentacion\Test Manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6A2E86-CF42-421E-9E57-8A797F0942EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448E3BBD-23FC-4FA1-BAC5-FED36732FA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{38327EC7-7A7F-423F-816A-788E1816B998}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -211,6 +211,204 @@
   <si>
     <t>Ejecutar backend</t>
   </si>
+  <si>
+    <t>SPRINT2 - 01</t>
+  </si>
+  <si>
+    <t>Obtener informacion de la cuenta</t>
+  </si>
+  <si>
+    <t>Consultar datos de la cuenta, como ser, CVU, alias y monto de dinero</t>
+  </si>
+  <si>
+    <t>Ejecutar backend en intellij y estar logueado</t>
+  </si>
+  <si>
+    <t>Seleccionar nueva peticion tipo GET</t>
+  </si>
+  <si>
+    <t>copiar URL "http://localhost:8084/account/1"</t>
+  </si>
+  <si>
+    <t>Respuesta 200 - OK</t>
+  </si>
+  <si>
+    <t>SPRINT2- 02</t>
+  </si>
+  <si>
+    <t>Obtener ultimos movimientos de la cuenta</t>
+  </si>
+  <si>
+    <t>Consultar sobre las ultimas 5 transacciones realizadas por el usuario</t>
+  </si>
+  <si>
+    <t>copiar URL "http://localhost:8084/account/transactions"</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 03</t>
+  </si>
+  <si>
+    <t>Update de usuario</t>
+  </si>
+  <si>
+    <t>Cambiar el telefono de un usuario</t>
+  </si>
+  <si>
+    <t>Loguearse con una cuenta a la app</t>
+  </si>
+  <si>
+    <t>Pegar token en "Authentication" -&gt; "Bearer Token" en postman</t>
+  </si>
+  <si>
+    <t>Seleccionar nueva peticion tipo PATCH</t>
+  </si>
+  <si>
+    <t>copiar URL "http://localhost:8084/user/update-user"</t>
+  </si>
+  <si>
+    <t>Agregar JSON con campos "name", "lastName", "username", "email" (con un numero distinto al registrado inicialmente), "phoneNumber" y "password"</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 04</t>
+  </si>
+  <si>
+    <t>Update de alias</t>
+  </si>
+  <si>
+    <t>Cambiar el alias que viene por defecto</t>
+  </si>
+  <si>
+    <t>copiar URL "http://localhost:8084/user/update-alias"</t>
+  </si>
+  <si>
+    <t>Agregar JSON con campo "alias" y su nuevo valor</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 05</t>
+  </si>
+  <si>
+    <t>Update Password</t>
+  </si>
+  <si>
+    <t>Cambiar password registrada inicialmente</t>
+  </si>
+  <si>
+    <t>copiar URL "http://localhost:8084/user/update-password"</t>
+  </si>
+  <si>
+    <t>Agregar JSON con campo "password" y "passwordRepeated"</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 06</t>
+  </si>
+  <si>
+    <t>Registro de una tarjeta</t>
+  </si>
+  <si>
+    <t>Agregar una tarjeta a una cuenta</t>
+  </si>
+  <si>
+    <t>copiar URL "http://localhost:8084/account/register-card"</t>
+  </si>
+  <si>
+    <t>Agregar JSON con campos "holder", "number", "expirationDate" y "cvv"</t>
+  </si>
+  <si>
+    <t>Respuesta 201 - CREATED</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 07</t>
+  </si>
+  <si>
+    <t>Registro de tarjeta fallido</t>
+  </si>
+  <si>
+    <t>Intentar registrar una tarjeta a una cuenta y que la tarjeta ya este registrada previamente</t>
+  </si>
+  <si>
+    <t>409 - CONFLICT</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 08</t>
+  </si>
+  <si>
+    <t>Intentar registrar una tarjeta con un campo incompleto</t>
+  </si>
+  <si>
+    <t>Agregar JSON con campos "holder", "number" (dejar en null), "expirationDate" y "cvv"</t>
+  </si>
+  <si>
+    <t>400 - Bad Request</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 09</t>
+  </si>
+  <si>
+    <t>Obtener tarjeta</t>
+  </si>
+  <si>
+    <t>Obtener tarjeta por ID</t>
+  </si>
+  <si>
+    <t>copiar URL "http://localhost:8084/account/card/1"</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 10</t>
+  </si>
+  <si>
+    <t>Obtener tarjeta fallido</t>
+  </si>
+  <si>
+    <t>Obtener tarjeta de ID inexistente</t>
+  </si>
+  <si>
+    <t>copiar URL "http://localhost:8084/account/card/3"</t>
+  </si>
+  <si>
+    <t>Respuesta 404 - Not Found</t>
+  </si>
+  <si>
+    <t>SPRINT - 11</t>
+  </si>
+  <si>
+    <t>Obtener lista de tarjetas</t>
+  </si>
+  <si>
+    <t>Obtener todas las tarjetas asociadas al usuario autenticado</t>
+  </si>
+  <si>
+    <t>copiar URL "http://localhost:8084/account/cards"</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 12</t>
+  </si>
+  <si>
+    <t>Obtener todas las tarjetas asociadas al usuario autenticado pero no haber registrado ninguna</t>
+  </si>
+  <si>
+    <t>Respuesta 200 - OK (array vacio)</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 13</t>
+  </si>
+  <si>
+    <t>Eliminar tarjeta</t>
+  </si>
+  <si>
+    <t>Eliminar tarjeta asociada a mi cuenta</t>
+  </si>
+  <si>
+    <t>Seleccionar nueva peticion tipo DELETE</t>
+  </si>
+  <si>
+    <t>copiar URL "http://localhost:8084/account/delete-card/1"</t>
+  </si>
+  <si>
+    <t>SPRINT2 - 14</t>
+  </si>
+  <si>
+    <t>Eliminar tarjeta de ID inexistente</t>
+  </si>
 </sst>
 </file>
 
@@ -261,7 +459,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -373,11 +571,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -400,6 +613,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -415,22 +646,40 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -769,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0435A08-4D3E-4B83-999E-9BEBF971F2FD}">
   <dimension ref="A1:Y872"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31:D35"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36:L107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.453125" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -789,36 +1038,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="8" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="1"/>
@@ -836,11 +1085,11 @@
       <c r="Y1" s="1"/>
     </row>
     <row r="2" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
@@ -850,10 +1099,10 @@
       <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -869,19 +1118,19 @@
       <c r="Y2" s="1"/>
     </row>
     <row r="3" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="8" t="s">
         <v>57</v>
       </c>
       <c r="F3" s="4">
@@ -891,16 +1140,16 @@
         <v>18</v>
       </c>
       <c r="H3" s="5"/>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="M3" s="1"/>
@@ -918,11 +1167,11 @@
       <c r="Y3" s="1"/>
     </row>
     <row r="4" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="14"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="4">
         <v>2</v>
       </c>
@@ -930,10 +1179,10 @@
         <v>22</v>
       </c>
       <c r="H4" s="5"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -949,11 +1198,11 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="14"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="4">
         <v>3</v>
       </c>
@@ -961,10 +1210,10 @@
         <v>23</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -980,11 +1229,11 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="14"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="4">
         <v>4</v>
       </c>
@@ -992,10 +1241,10 @@
         <v>24</v>
       </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1011,11 +1260,11 @@
       <c r="Y6" s="1"/>
     </row>
     <row r="7" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="4">
         <v>5</v>
       </c>
@@ -1025,10 +1274,10 @@
       <c r="H7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1044,11 +1293,11 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="4">
         <v>6</v>
       </c>
@@ -1058,10 +1307,10 @@
       <c r="H8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -1077,11 +1326,11 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="4">
         <v>7</v>
       </c>
@@ -1091,10 +1340,10 @@
       <c r="H9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1110,11 +1359,11 @@
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="4">
         <v>8</v>
       </c>
@@ -1124,10 +1373,10 @@
       <c r="H10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1143,19 +1392,19 @@
       <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="4">
@@ -1165,16 +1414,16 @@
         <v>18</v>
       </c>
       <c r="H11" s="5"/>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="M11" s="1"/>
@@ -1192,11 +1441,11 @@
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="14"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="4">
         <v>2</v>
       </c>
@@ -1204,10 +1453,10 @@
         <v>22</v>
       </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1223,11 +1472,11 @@
       <c r="Y12" s="1"/>
     </row>
     <row r="13" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="14"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="4">
         <v>3</v>
       </c>
@@ -1235,10 +1484,10 @@
         <v>23</v>
       </c>
       <c r="H13" s="5"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1254,11 +1503,11 @@
       <c r="Y13" s="1"/>
     </row>
     <row r="14" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="4">
         <v>4</v>
       </c>
@@ -1266,10 +1515,10 @@
         <v>36</v>
       </c>
       <c r="H14" s="5"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1285,11 +1534,11 @@
       <c r="Y14" s="1"/>
     </row>
     <row r="15" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="15"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="4">
         <v>5</v>
       </c>
@@ -1299,10 +1548,10 @@
       <c r="H15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1318,19 +1567,19 @@
       <c r="Y15" s="1"/>
     </row>
     <row r="16" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="4">
@@ -1340,16 +1589,16 @@
         <v>18</v>
       </c>
       <c r="H16" s="5"/>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="16" t="s">
+      <c r="J16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="16" t="s">
+      <c r="K16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="16" t="s">
+      <c r="L16" s="8" t="s">
         <v>21</v>
       </c>
       <c r="M16" s="1"/>
@@ -1367,11 +1616,11 @@
       <c r="Y16" s="1"/>
     </row>
     <row r="17" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="4">
         <v>2</v>
       </c>
@@ -1379,10 +1628,10 @@
         <v>22</v>
       </c>
       <c r="H17" s="5"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1398,11 +1647,11 @@
       <c r="Y17" s="1"/>
     </row>
     <row r="18" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="14"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="4">
         <v>3</v>
       </c>
@@ -1410,10 +1659,10 @@
         <v>23</v>
       </c>
       <c r="H18" s="5"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1429,11 +1678,11 @@
       <c r="Y18" s="1"/>
     </row>
     <row r="19" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="14"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="4">
         <v>4</v>
       </c>
@@ -1441,10 +1690,10 @@
         <v>41</v>
       </c>
       <c r="H19" s="5"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1460,11 +1709,11 @@
       <c r="Y19" s="1"/>
     </row>
     <row r="20" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="15"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="4">
         <v>5</v>
       </c>
@@ -1474,10 +1723,10 @@
       <c r="H20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1493,19 +1742,19 @@
       <c r="Y20" s="1"/>
     </row>
     <row r="21" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F21" s="4">
@@ -1515,16 +1764,16 @@
         <v>18</v>
       </c>
       <c r="H21" s="5"/>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="J21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="16" t="s">
+      <c r="K21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="8" t="s">
         <v>21</v>
       </c>
       <c r="M21" s="1"/>
@@ -1542,11 +1791,11 @@
       <c r="Y21" s="1"/>
     </row>
     <row r="22" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="4">
         <v>2</v>
       </c>
@@ -1554,10 +1803,10 @@
         <v>22</v>
       </c>
       <c r="H22" s="5"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -1573,11 +1822,11 @@
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="14"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="4">
         <v>3</v>
       </c>
@@ -1585,10 +1834,10 @@
         <v>23</v>
       </c>
       <c r="H23" s="5"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1604,11 +1853,11 @@
       <c r="Y23" s="1"/>
     </row>
     <row r="24" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="14"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="6">
         <v>4</v>
       </c>
@@ -1616,10 +1865,10 @@
         <v>46</v>
       </c>
       <c r="H24" s="5"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1635,11 +1884,11 @@
       <c r="Y24" s="1"/>
     </row>
     <row r="25" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="15"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="4">
         <v>5</v>
       </c>
@@ -1649,10 +1898,10 @@
       <c r="H25" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1668,19 +1917,19 @@
       <c r="Y25" s="1"/>
     </row>
     <row r="26" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F26" s="4">
@@ -1690,16 +1939,16 @@
         <v>18</v>
       </c>
       <c r="H26" s="5"/>
-      <c r="I26" s="16" t="s">
+      <c r="I26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="16" t="s">
+      <c r="J26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K26" s="16" t="s">
+      <c r="K26" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L26" s="16" t="s">
+      <c r="L26" s="8" t="s">
         <v>21</v>
       </c>
       <c r="M26" s="1"/>
@@ -1717,11 +1966,11 @@
       <c r="Y26" s="1"/>
     </row>
     <row r="27" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="14"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
       <c r="F27" s="4">
         <v>2</v>
       </c>
@@ -1729,10 +1978,10 @@
         <v>50</v>
       </c>
       <c r="H27" s="5"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -1748,11 +1997,11 @@
       <c r="Y27" s="1"/>
     </row>
     <row r="28" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="14"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
       <c r="F28" s="4">
         <v>3</v>
       </c>
@@ -1760,10 +2009,10 @@
         <v>23</v>
       </c>
       <c r="H28" s="5"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -1779,11 +2028,11 @@
       <c r="Y28" s="1"/>
     </row>
     <row r="29" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
       <c r="F29" s="4">
         <v>4</v>
       </c>
@@ -1791,10 +2040,10 @@
         <v>51</v>
       </c>
       <c r="H29" s="5"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -1810,11 +2059,11 @@
       <c r="Y29" s="1"/>
     </row>
     <row r="30" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="15"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="6">
         <v>5</v>
       </c>
@@ -1824,10 +2073,10 @@
       <c r="H30" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -1843,19 +2092,19 @@
       <c r="Y30" s="1"/>
     </row>
     <row r="31" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F31" s="4">
@@ -1865,16 +2114,16 @@
         <v>18</v>
       </c>
       <c r="H31" s="5"/>
-      <c r="I31" s="16" t="s">
+      <c r="I31" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J31" s="16" t="s">
+      <c r="J31" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K31" s="16" t="s">
+      <c r="K31" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L31" s="16" t="s">
+      <c r="L31" s="8" t="s">
         <v>21</v>
       </c>
       <c r="M31" s="1"/>
@@ -1892,11 +2141,11 @@
       <c r="Y31" s="1"/>
     </row>
     <row r="32" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="14"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
       <c r="F32" s="4">
         <v>2</v>
       </c>
@@ -1904,10 +2153,10 @@
         <v>50</v>
       </c>
       <c r="H32" s="5"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -1923,11 +2172,11 @@
       <c r="Y32" s="1"/>
     </row>
     <row r="33" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="14"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
       <c r="F33" s="4">
         <v>3</v>
       </c>
@@ -1935,10 +2184,10 @@
         <v>23</v>
       </c>
       <c r="H33" s="5"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -1954,11 +2203,11 @@
       <c r="Y33" s="1"/>
     </row>
     <row r="34" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="14"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
       <c r="F34" s="4">
         <v>4</v>
       </c>
@@ -1966,10 +2215,10 @@
         <v>56</v>
       </c>
       <c r="H34" s="5"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -1985,11 +2234,11 @@
       <c r="Y34" s="1"/>
     </row>
     <row r="35" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="15"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
       <c r="F35" s="4">
         <v>5</v>
       </c>
@@ -1999,10 +2248,10 @@
       <c r="H35" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -2018,18 +2267,40 @@
       <c r="Y35" s="1"/>
     </row>
     <row r="36" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
+      <c r="A36" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="19">
+        <v>1</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H36" s="20"/>
+      <c r="I36" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -2045,18 +2316,22 @@
       <c r="Y36" s="1"/>
     </row>
     <row r="37" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="21">
+        <v>2</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H37" s="22"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -2072,18 +2347,24 @@
       <c r="Y37" s="1"/>
     </row>
     <row r="38" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="21">
+        <v>3</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -2099,18 +2380,32 @@
       <c r="Y38" s="1"/>
     </row>
     <row r="39" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
+      <c r="A39" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="23">
+        <v>1</v>
+      </c>
+      <c r="G39" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H39" s="22"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
@@ -2126,18 +2421,22 @@
       <c r="Y39" s="1"/>
     </row>
     <row r="40" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="23">
+        <v>2</v>
+      </c>
+      <c r="G40" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" s="22"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -2153,18 +2452,24 @@
       <c r="Y40" s="1"/>
     </row>
     <row r="41" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="23">
+        <v>3</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
@@ -2180,18 +2485,32 @@
       <c r="Y41" s="1"/>
     </row>
     <row r="42" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
+      <c r="A42" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="21">
+        <v>1</v>
+      </c>
+      <c r="G42" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H42" s="22"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
@@ -2207,18 +2526,22 @@
       <c r="Y42" s="1"/>
     </row>
     <row r="43" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="21">
+        <v>2</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H43" s="22"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
@@ -2234,18 +2557,30 @@
       <c r="Y43" s="1"/>
     </row>
     <row r="44" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="21">
+        <v>3</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H44" s="22"/>
+      <c r="I44" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
@@ -2261,18 +2596,22 @@
       <c r="Y44" s="1"/>
     </row>
     <row r="45" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="21">
+        <v>4</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H45" s="22"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
@@ -2288,18 +2627,22 @@
       <c r="Y45" s="1"/>
     </row>
     <row r="46" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="23">
+        <v>5</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H46" s="22"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -2315,18 +2658,24 @@
       <c r="Y46" s="1"/>
     </row>
     <row r="47" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="21">
+        <v>6</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
@@ -2342,18 +2691,32 @@
       <c r="Y47" s="1"/>
     </row>
     <row r="48" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
+      <c r="A48" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48" s="21">
+        <v>1</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H48" s="22"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -2369,18 +2732,22 @@
       <c r="Y48" s="1"/>
     </row>
     <row r="49" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="21">
+        <v>2</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H49" s="22"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
@@ -2396,18 +2763,22 @@
       <c r="Y49" s="1"/>
     </row>
     <row r="50" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="21">
+        <v>3</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H50" s="22"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
@@ -2423,18 +2794,22 @@
       <c r="Y50" s="1"/>
     </row>
     <row r="51" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="21">
+        <v>4</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="H51" s="22"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
@@ -2450,18 +2825,30 @@
       <c r="Y51" s="1"/>
     </row>
     <row r="52" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="21">
+        <v>5</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H52" s="22"/>
+      <c r="I52" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L52" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -2477,18 +2864,24 @@
       <c r="Y52" s="1"/>
     </row>
     <row r="53" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="21">
+        <v>6</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H53" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -2504,18 +2897,32 @@
       <c r="Y53" s="1"/>
     </row>
     <row r="54" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
+      <c r="A54" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F54" s="21">
+        <v>1</v>
+      </c>
+      <c r="G54" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H54" s="22"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
@@ -2531,18 +2938,22 @@
       <c r="Y54" s="1"/>
     </row>
     <row r="55" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="21">
+        <v>2</v>
+      </c>
+      <c r="G55" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H55" s="22"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
@@ -2558,18 +2969,22 @@
       <c r="Y55" s="1"/>
     </row>
     <row r="56" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="21">
+        <v>3</v>
+      </c>
+      <c r="G56" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H56" s="22"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
@@ -2585,18 +3000,22 @@
       <c r="Y56" s="1"/>
     </row>
     <row r="57" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="23">
+        <v>4</v>
+      </c>
+      <c r="G57" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H57" s="22"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
@@ -2612,18 +3031,22 @@
       <c r="Y57" s="1"/>
     </row>
     <row r="58" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="21">
+        <v>5</v>
+      </c>
+      <c r="G58" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="H58" s="22"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
@@ -2639,18 +3062,24 @@
       <c r="Y58" s="1"/>
     </row>
     <row r="59" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="21">
+        <v>6</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H59" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
@@ -2666,18 +3095,40 @@
       <c r="Y59" s="1"/>
     </row>
     <row r="60" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
+      <c r="A60" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E60" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F60" s="21">
+        <v>1</v>
+      </c>
+      <c r="G60" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H60" s="22"/>
+      <c r="I60" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L60" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
@@ -2693,18 +3144,22 @@
       <c r="Y60" s="1"/>
     </row>
     <row r="61" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="21">
+        <v>2</v>
+      </c>
+      <c r="G61" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H61" s="22"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
@@ -2720,18 +3175,22 @@
       <c r="Y61" s="1"/>
     </row>
     <row r="62" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="21">
+        <v>3</v>
+      </c>
+      <c r="G62" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H62" s="22"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
@@ -2747,18 +3206,22 @@
       <c r="Y62" s="1"/>
     </row>
     <row r="63" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="23">
+        <v>4</v>
+      </c>
+      <c r="G63" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H63" s="22"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
@@ -2774,18 +3237,22 @@
       <c r="Y63" s="1"/>
     </row>
     <row r="64" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="21">
+        <v>5</v>
+      </c>
+      <c r="G64" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H64" s="22"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
@@ -2801,18 +3268,24 @@
       <c r="Y64" s="1"/>
     </row>
     <row r="65" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
+      <c r="A65" s="27"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="21">
+        <v>6</v>
+      </c>
+      <c r="G65" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H65" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
@@ -2828,18 +3301,32 @@
       <c r="Y65" s="1"/>
     </row>
     <row r="66" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
+      <c r="A66" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E66" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F66" s="21">
+        <v>1</v>
+      </c>
+      <c r="G66" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H66" s="22"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
@@ -2855,18 +3342,22 @@
       <c r="Y66" s="1"/>
     </row>
     <row r="67" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="21">
+        <v>2</v>
+      </c>
+      <c r="G67" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H67" s="22"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
@@ -2882,18 +3373,30 @@
       <c r="Y67" s="1"/>
     </row>
     <row r="68" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
+      <c r="A68" s="26"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="21">
+        <v>3</v>
+      </c>
+      <c r="G68" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H68" s="22"/>
+      <c r="I68" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J68" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K68" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L68" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
@@ -2909,18 +3412,22 @@
       <c r="Y68" s="1"/>
     </row>
     <row r="69" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
+      <c r="A69" s="26"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="21">
+        <v>4</v>
+      </c>
+      <c r="G69" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H69" s="22"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
@@ -2936,18 +3443,22 @@
       <c r="Y69" s="1"/>
     </row>
     <row r="70" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="21">
+        <v>5</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H70" s="22"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
@@ -2963,18 +3474,24 @@
       <c r="Y70" s="1"/>
     </row>
     <row r="71" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
+      <c r="A71" s="27"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="21">
+        <v>6</v>
+      </c>
+      <c r="G71" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H71" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
@@ -2990,18 +3507,32 @@
       <c r="Y71" s="1"/>
     </row>
     <row r="72" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
+      <c r="A72" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B72" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D72" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E72" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F72" s="21">
+        <v>1</v>
+      </c>
+      <c r="G72" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H72" s="22"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
@@ -3017,18 +3548,22 @@
       <c r="Y72" s="1"/>
     </row>
     <row r="73" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
+      <c r="A73" s="26"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="21">
+        <v>2</v>
+      </c>
+      <c r="G73" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H73" s="22"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
@@ -3044,18 +3579,22 @@
       <c r="Y73" s="1"/>
     </row>
     <row r="74" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
+      <c r="A74" s="26"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="21">
+        <v>3</v>
+      </c>
+      <c r="G74" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H74" s="22"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="9"/>
+      <c r="K74" s="9"/>
+      <c r="L74" s="9"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
@@ -3071,18 +3610,22 @@
       <c r="Y74" s="1"/>
     </row>
     <row r="75" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
+      <c r="A75" s="26"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="21">
+        <v>4</v>
+      </c>
+      <c r="G75" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H75" s="22"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
@@ -3098,18 +3641,30 @@
       <c r="Y75" s="1"/>
     </row>
     <row r="76" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
+      <c r="A76" s="26"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="21">
+        <v>5</v>
+      </c>
+      <c r="G76" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="H76" s="22"/>
+      <c r="I76" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J76" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K76" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L76" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
@@ -3125,18 +3680,24 @@
       <c r="Y76" s="1"/>
     </row>
     <row r="77" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
+      <c r="A77" s="27"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="30"/>
+      <c r="F77" s="21">
+        <v>6</v>
+      </c>
+      <c r="G77" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H77" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
@@ -3152,18 +3713,32 @@
       <c r="Y77" s="1"/>
     </row>
     <row r="78" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="L78" s="1"/>
+      <c r="A78" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D78" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E78" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F78" s="21">
+        <v>1</v>
+      </c>
+      <c r="G78" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H78" s="22"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
@@ -3179,18 +3754,22 @@
       <c r="Y78" s="1"/>
     </row>
     <row r="79" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
+      <c r="A79" s="26"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="21">
+        <v>2</v>
+      </c>
+      <c r="G79" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H79" s="22"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="9"/>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -3206,18 +3785,22 @@
       <c r="Y79" s="1"/>
     </row>
     <row r="80" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
+      <c r="A80" s="26"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="21">
+        <v>3</v>
+      </c>
+      <c r="G80" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H80" s="22"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="9"/>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
@@ -3233,18 +3816,22 @@
       <c r="Y80" s="1"/>
     </row>
     <row r="81" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
+      <c r="A81" s="26"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="21">
+        <v>4</v>
+      </c>
+      <c r="G81" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="H81" s="22"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="9"/>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
@@ -3260,18 +3847,24 @@
       <c r="Y81" s="1"/>
     </row>
     <row r="82" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1"/>
-      <c r="K82" s="1"/>
-      <c r="L82" s="1"/>
+      <c r="A82" s="27"/>
+      <c r="B82" s="30"/>
+      <c r="C82" s="30"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="30"/>
+      <c r="F82" s="21">
+        <v>5</v>
+      </c>
+      <c r="G82" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H82" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I82" s="9"/>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="9"/>
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
@@ -3287,18 +3880,32 @@
       <c r="Y82" s="1"/>
     </row>
     <row r="83" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
+      <c r="A83" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B83" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D83" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E83" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F83" s="21">
+        <v>1</v>
+      </c>
+      <c r="G83" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H83" s="22"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="10"/>
+      <c r="K83" s="10"/>
+      <c r="L83" s="10"/>
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
@@ -3314,18 +3921,30 @@
       <c r="Y83" s="1"/>
     </row>
     <row r="84" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
-      <c r="J84" s="1"/>
-      <c r="K84" s="1"/>
-      <c r="L84" s="1"/>
+      <c r="A84" s="26"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="21">
+        <v>2</v>
+      </c>
+      <c r="G84" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H84" s="22"/>
+      <c r="I84" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J84" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K84" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L84" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
@@ -3341,18 +3960,22 @@
       <c r="Y84" s="1"/>
     </row>
     <row r="85" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-      <c r="K85" s="1"/>
-      <c r="L85" s="1"/>
+      <c r="A85" s="26"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="21">
+        <v>3</v>
+      </c>
+      <c r="G85" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H85" s="22"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="9"/>
+      <c r="L85" s="9"/>
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
@@ -3368,18 +3991,22 @@
       <c r="Y85" s="1"/>
     </row>
     <row r="86" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
-      <c r="L86" s="1"/>
+      <c r="A86" s="26"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="21">
+        <v>4</v>
+      </c>
+      <c r="G86" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="H86" s="22"/>
+      <c r="I86" s="9"/>
+      <c r="J86" s="9"/>
+      <c r="K86" s="9"/>
+      <c r="L86" s="9"/>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
@@ -3395,18 +4022,24 @@
       <c r="Y86" s="1"/>
     </row>
     <row r="87" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
-      <c r="L87" s="1"/>
+      <c r="A87" s="27"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="21">
+        <v>5</v>
+      </c>
+      <c r="G87" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H87" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I87" s="9"/>
+      <c r="J87" s="9"/>
+      <c r="K87" s="9"/>
+      <c r="L87" s="9"/>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
@@ -3422,18 +4055,32 @@
       <c r="Y87" s="1"/>
     </row>
     <row r="88" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-      <c r="K88" s="1"/>
-      <c r="L88" s="1"/>
+      <c r="A88" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B88" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D88" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E88" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F88" s="21">
+        <v>1</v>
+      </c>
+      <c r="G88" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H88" s="22"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="9"/>
+      <c r="K88" s="9"/>
+      <c r="L88" s="9"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
@@ -3449,18 +4096,22 @@
       <c r="Y88" s="1"/>
     </row>
     <row r="89" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="1"/>
-      <c r="J89" s="1"/>
-      <c r="K89" s="1"/>
-      <c r="L89" s="1"/>
+      <c r="A89" s="26"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="21">
+        <v>2</v>
+      </c>
+      <c r="G89" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H89" s="22"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+      <c r="K89" s="9"/>
+      <c r="L89" s="9"/>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
@@ -3476,18 +4127,22 @@
       <c r="Y89" s="1"/>
     </row>
     <row r="90" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
-      <c r="L90" s="1"/>
+      <c r="A90" s="26"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="21">
+        <v>3</v>
+      </c>
+      <c r="G90" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H90" s="22"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="9"/>
+      <c r="K90" s="9"/>
+      <c r="L90" s="9"/>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
@@ -3503,18 +4158,22 @@
       <c r="Y90" s="1"/>
     </row>
     <row r="91" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-      <c r="K91" s="1"/>
-      <c r="L91" s="1"/>
+      <c r="A91" s="26"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="29"/>
+      <c r="E91" s="29"/>
+      <c r="F91" s="21">
+        <v>4</v>
+      </c>
+      <c r="G91" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H91" s="22"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10"/>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
@@ -3530,18 +4189,32 @@
       <c r="Y91" s="1"/>
     </row>
     <row r="92" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
-      <c r="L92" s="1"/>
+      <c r="A92" s="27"/>
+      <c r="B92" s="30"/>
+      <c r="C92" s="30"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="30"/>
+      <c r="F92" s="21">
+        <v>5</v>
+      </c>
+      <c r="G92" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H92" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I92" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J92" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K92" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L92" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
@@ -3557,18 +4230,32 @@
       <c r="Y92" s="1"/>
     </row>
     <row r="93" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-      <c r="K93" s="1"/>
-      <c r="L93" s="1"/>
+      <c r="A93" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B93" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D93" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E93" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F93" s="21">
+        <v>1</v>
+      </c>
+      <c r="G93" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H93" s="22"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="9"/>
+      <c r="K93" s="9"/>
+      <c r="L93" s="9"/>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
@@ -3584,18 +4271,22 @@
       <c r="Y93" s="1"/>
     </row>
     <row r="94" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="1"/>
-      <c r="J94" s="1"/>
-      <c r="K94" s="1"/>
-      <c r="L94" s="1"/>
+      <c r="A94" s="26"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="21">
+        <v>2</v>
+      </c>
+      <c r="G94" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H94" s="22"/>
+      <c r="I94" s="9"/>
+      <c r="J94" s="9"/>
+      <c r="K94" s="9"/>
+      <c r="L94" s="9"/>
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
@@ -3611,18 +4302,22 @@
       <c r="Y94" s="1"/>
     </row>
     <row r="95" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-      <c r="K95" s="1"/>
-      <c r="L95" s="1"/>
+      <c r="A95" s="26"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="29"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="21">
+        <v>3</v>
+      </c>
+      <c r="G95" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H95" s="22"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="9"/>
+      <c r="L95" s="9"/>
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
@@ -3638,18 +4333,22 @@
       <c r="Y95" s="1"/>
     </row>
     <row r="96" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
-      <c r="J96" s="1"/>
-      <c r="K96" s="1"/>
-      <c r="L96" s="1"/>
+      <c r="A96" s="26"/>
+      <c r="B96" s="29"/>
+      <c r="C96" s="29"/>
+      <c r="D96" s="29"/>
+      <c r="E96" s="29"/>
+      <c r="F96" s="21">
+        <v>4</v>
+      </c>
+      <c r="G96" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H96" s="22"/>
+      <c r="I96" s="9"/>
+      <c r="J96" s="9"/>
+      <c r="K96" s="9"/>
+      <c r="L96" s="9"/>
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
@@ -3665,18 +4364,24 @@
       <c r="Y96" s="1"/>
     </row>
     <row r="97" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
-      <c r="K97" s="1"/>
-      <c r="L97" s="1"/>
+      <c r="A97" s="27"/>
+      <c r="B97" s="30"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="30"/>
+      <c r="F97" s="21">
+        <v>5</v>
+      </c>
+      <c r="G97" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H97" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I97" s="9"/>
+      <c r="J97" s="9"/>
+      <c r="K97" s="9"/>
+      <c r="L97" s="9"/>
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
@@ -3692,18 +4397,32 @@
       <c r="Y97" s="1"/>
     </row>
     <row r="98" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
-      <c r="I98" s="1"/>
-      <c r="J98" s="1"/>
-      <c r="K98" s="1"/>
-      <c r="L98" s="1"/>
+      <c r="A98" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B98" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C98" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D98" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="E98" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F98" s="23">
+        <v>1</v>
+      </c>
+      <c r="G98" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H98" s="24"/>
+      <c r="I98" s="9"/>
+      <c r="J98" s="9"/>
+      <c r="K98" s="9"/>
+      <c r="L98" s="9"/>
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
@@ -3719,18 +4438,22 @@
       <c r="Y98" s="1"/>
     </row>
     <row r="99" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
-      <c r="K99" s="1"/>
-      <c r="L99" s="1"/>
+      <c r="A99" s="26"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="29"/>
+      <c r="D99" s="29"/>
+      <c r="E99" s="29"/>
+      <c r="F99" s="23">
+        <v>2</v>
+      </c>
+      <c r="G99" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H99" s="24"/>
+      <c r="I99" s="10"/>
+      <c r="J99" s="10"/>
+      <c r="K99" s="10"/>
+      <c r="L99" s="10"/>
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
@@ -3746,18 +4469,30 @@
       <c r="Y99" s="1"/>
     </row>
     <row r="100" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
+      <c r="A100" s="26"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="29"/>
+      <c r="E100" s="29"/>
+      <c r="F100" s="23">
+        <v>3</v>
+      </c>
+      <c r="G100" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H100" s="24"/>
+      <c r="I100" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J100" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K100" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L100" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
@@ -3773,18 +4508,22 @@
       <c r="Y100" s="1"/>
     </row>
     <row r="101" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
-      <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
+      <c r="A101" s="26"/>
+      <c r="B101" s="29"/>
+      <c r="C101" s="29"/>
+      <c r="D101" s="29"/>
+      <c r="E101" s="29"/>
+      <c r="F101" s="23">
+        <v>4</v>
+      </c>
+      <c r="G101" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H101" s="24"/>
+      <c r="I101" s="9"/>
+      <c r="J101" s="9"/>
+      <c r="K101" s="9"/>
+      <c r="L101" s="9"/>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
@@ -3800,18 +4539,24 @@
       <c r="Y101" s="1"/>
     </row>
     <row r="102" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-      <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
+      <c r="A102" s="27"/>
+      <c r="B102" s="30"/>
+      <c r="C102" s="30"/>
+      <c r="D102" s="30"/>
+      <c r="E102" s="30"/>
+      <c r="F102" s="23">
+        <v>5</v>
+      </c>
+      <c r="G102" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H102" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="I102" s="9"/>
+      <c r="J102" s="9"/>
+      <c r="K102" s="9"/>
+      <c r="L102" s="9"/>
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1"/>
@@ -3827,18 +4572,32 @@
       <c r="Y102" s="1"/>
     </row>
     <row r="103" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="I103" s="1"/>
-      <c r="J103" s="1"/>
-      <c r="K103" s="1"/>
-      <c r="L103" s="1"/>
+      <c r="A103" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B103" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D103" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E103" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F103" s="23">
+        <v>1</v>
+      </c>
+      <c r="G103" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H103" s="24"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9"/>
+      <c r="K103" s="9"/>
+      <c r="L103" s="9"/>
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
       <c r="O103" s="1"/>
@@ -3854,18 +4613,22 @@
       <c r="Y103" s="1"/>
     </row>
     <row r="104" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1"/>
-      <c r="J104" s="1"/>
-      <c r="K104" s="1"/>
-      <c r="L104" s="1"/>
+      <c r="A104" s="26"/>
+      <c r="B104" s="29"/>
+      <c r="C104" s="29"/>
+      <c r="D104" s="29"/>
+      <c r="E104" s="29"/>
+      <c r="F104" s="23">
+        <v>2</v>
+      </c>
+      <c r="G104" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H104" s="24"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="9"/>
+      <c r="K104" s="9"/>
+      <c r="L104" s="9"/>
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
       <c r="O104" s="1"/>
@@ -3881,18 +4644,22 @@
       <c r="Y104" s="1"/>
     </row>
     <row r="105" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
-      <c r="I105" s="1"/>
-      <c r="J105" s="1"/>
-      <c r="K105" s="1"/>
-      <c r="L105" s="1"/>
+      <c r="A105" s="26"/>
+      <c r="B105" s="29"/>
+      <c r="C105" s="29"/>
+      <c r="D105" s="29"/>
+      <c r="E105" s="29"/>
+      <c r="F105" s="23">
+        <v>3</v>
+      </c>
+      <c r="G105" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H105" s="24"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
+      <c r="L105" s="9"/>
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
       <c r="O105" s="1"/>
@@ -3908,18 +4675,22 @@
       <c r="Y105" s="1"/>
     </row>
     <row r="106" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
-      <c r="H106" s="1"/>
-      <c r="I106" s="1"/>
-      <c r="J106" s="1"/>
-      <c r="K106" s="1"/>
-      <c r="L106" s="1"/>
+      <c r="A106" s="26"/>
+      <c r="B106" s="29"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="29"/>
+      <c r="E106" s="29"/>
+      <c r="F106" s="23">
+        <v>4</v>
+      </c>
+      <c r="G106" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H106" s="24"/>
+      <c r="I106" s="9"/>
+      <c r="J106" s="9"/>
+      <c r="K106" s="9"/>
+      <c r="L106" s="9"/>
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
       <c r="O106" s="1"/>
@@ -3935,18 +4706,24 @@
       <c r="Y106" s="1"/>
     </row>
     <row r="107" spans="1:25" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-      <c r="F107" s="1"/>
-      <c r="G107" s="1"/>
-      <c r="H107" s="1"/>
-      <c r="I107" s="1"/>
-      <c r="J107" s="1"/>
-      <c r="K107" s="1"/>
-      <c r="L107" s="1"/>
+      <c r="A107" s="27"/>
+      <c r="B107" s="30"/>
+      <c r="C107" s="30"/>
+      <c r="D107" s="30"/>
+      <c r="E107" s="30"/>
+      <c r="F107" s="23">
+        <v>5</v>
+      </c>
+      <c r="G107" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H107" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10"/>
+      <c r="K107" s="10"/>
+      <c r="L107" s="10"/>
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
       <c r="O107" s="1"/>
@@ -24617,56 +25394,113 @@
       <c r="Y872" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="I31:I35"/>
-    <mergeCell ref="J31:J35"/>
-    <mergeCell ref="K31:K35"/>
-    <mergeCell ref="L31:L35"/>
-    <mergeCell ref="I26:I30"/>
-    <mergeCell ref="J26:J30"/>
-    <mergeCell ref="K26:K30"/>
-    <mergeCell ref="L26:L30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="D31:D35"/>
-    <mergeCell ref="E31:E35"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="L21:L25"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="E26:E30"/>
-    <mergeCell ref="I16:I20"/>
-    <mergeCell ref="J16:J20"/>
-    <mergeCell ref="K16:K20"/>
-    <mergeCell ref="L16:L20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="E21:E25"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="J11:J15"/>
-    <mergeCell ref="K11:K15"/>
-    <mergeCell ref="L11:L15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="D16:D20"/>
-    <mergeCell ref="E16:E20"/>
-    <mergeCell ref="I3:I10"/>
-    <mergeCell ref="J3:J10"/>
-    <mergeCell ref="K3:K10"/>
-    <mergeCell ref="L3:L10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:E15"/>
+  <mergeCells count="170">
+    <mergeCell ref="I100:I107"/>
+    <mergeCell ref="J100:J107"/>
+    <mergeCell ref="K100:K107"/>
+    <mergeCell ref="L100:L107"/>
+    <mergeCell ref="I84:I91"/>
+    <mergeCell ref="J84:J91"/>
+    <mergeCell ref="K84:K91"/>
+    <mergeCell ref="L84:L91"/>
+    <mergeCell ref="I92:I99"/>
+    <mergeCell ref="J92:J99"/>
+    <mergeCell ref="K92:K99"/>
+    <mergeCell ref="L92:L99"/>
+    <mergeCell ref="I68:I75"/>
+    <mergeCell ref="J68:J75"/>
+    <mergeCell ref="K68:K75"/>
+    <mergeCell ref="L68:L75"/>
+    <mergeCell ref="I76:I83"/>
+    <mergeCell ref="J76:J83"/>
+    <mergeCell ref="K76:K83"/>
+    <mergeCell ref="L76:L83"/>
+    <mergeCell ref="I52:I59"/>
+    <mergeCell ref="J52:J59"/>
+    <mergeCell ref="K52:K59"/>
+    <mergeCell ref="L52:L59"/>
+    <mergeCell ref="I60:I67"/>
+    <mergeCell ref="J60:J67"/>
+    <mergeCell ref="K60:K67"/>
+    <mergeCell ref="L60:L67"/>
+    <mergeCell ref="I36:I43"/>
+    <mergeCell ref="J36:J43"/>
+    <mergeCell ref="K36:K43"/>
+    <mergeCell ref="L36:L43"/>
+    <mergeCell ref="I44:I51"/>
+    <mergeCell ref="J44:J51"/>
+    <mergeCell ref="K44:K51"/>
+    <mergeCell ref="L44:L51"/>
+    <mergeCell ref="A103:A107"/>
+    <mergeCell ref="B103:B107"/>
+    <mergeCell ref="C103:C107"/>
+    <mergeCell ref="D103:D107"/>
+    <mergeCell ref="E103:E107"/>
+    <mergeCell ref="A98:A102"/>
+    <mergeCell ref="B98:B102"/>
+    <mergeCell ref="C98:C102"/>
+    <mergeCell ref="D98:D102"/>
+    <mergeCell ref="E98:E102"/>
+    <mergeCell ref="A93:A97"/>
+    <mergeCell ref="B93:B97"/>
+    <mergeCell ref="C93:C97"/>
+    <mergeCell ref="D93:D97"/>
+    <mergeCell ref="E93:E97"/>
+    <mergeCell ref="A88:A92"/>
+    <mergeCell ref="B88:B92"/>
+    <mergeCell ref="C88:C92"/>
+    <mergeCell ref="D88:D92"/>
+    <mergeCell ref="E88:E92"/>
+    <mergeCell ref="A83:A87"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="D83:D87"/>
+    <mergeCell ref="E83:E87"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="D78:D82"/>
+    <mergeCell ref="E78:E82"/>
+    <mergeCell ref="A72:A77"/>
+    <mergeCell ref="B72:B77"/>
+    <mergeCell ref="C72:C77"/>
+    <mergeCell ref="D72:D77"/>
+    <mergeCell ref="E72:E77"/>
+    <mergeCell ref="A66:A71"/>
+    <mergeCell ref="B66:B71"/>
+    <mergeCell ref="C66:C71"/>
+    <mergeCell ref="D66:D71"/>
+    <mergeCell ref="E66:E71"/>
+    <mergeCell ref="A60:A65"/>
+    <mergeCell ref="B60:B65"/>
+    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="D60:D65"/>
+    <mergeCell ref="E60:E65"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="B54:B59"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="E54:E59"/>
+    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="B48:B53"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="D48:D53"/>
+    <mergeCell ref="E48:E53"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
@@ -24682,6 +25516,55 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I3:I10"/>
+    <mergeCell ref="J3:J10"/>
+    <mergeCell ref="K3:K10"/>
+    <mergeCell ref="L3:L10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="J11:J15"/>
+    <mergeCell ref="K11:K15"/>
+    <mergeCell ref="L11:L15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="D16:D20"/>
+    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="I16:I20"/>
+    <mergeCell ref="J16:J20"/>
+    <mergeCell ref="K16:K20"/>
+    <mergeCell ref="L16:L20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="E21:E25"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="L21:L25"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="D31:D35"/>
+    <mergeCell ref="E31:E35"/>
+    <mergeCell ref="I31:I35"/>
+    <mergeCell ref="J31:J35"/>
+    <mergeCell ref="K31:K35"/>
+    <mergeCell ref="L31:L35"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="K26:K30"/>
+    <mergeCell ref="L26:L30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>